<commit_message>
test(dev): adjust file custom_class to get symbol list
</commit_message>
<xml_diff>
--- a/reports/ativos_resultado.xlsx
+++ b/reports/ativos_resultado.xlsx
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="J2" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="3">
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="J3" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="4">
@@ -588,7 +588,7 @@
         </is>
       </c>
       <c r="J4" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="5">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="J5" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="6">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="J6" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="7">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="J7" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="8">
@@ -724,7 +724,7 @@
         </is>
       </c>
       <c r="J8" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="9">
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="J9" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="10">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="J10" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="11">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="J11" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="12">
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="J12" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="13">
@@ -894,7 +894,7 @@
         </is>
       </c>
       <c r="J13" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="14">
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="J14" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="15">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="J15" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="16">
@@ -996,7 +996,7 @@
         </is>
       </c>
       <c r="J16" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="17">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="J17" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="18">
@@ -1064,7 +1064,7 @@
         </is>
       </c>
       <c r="J18" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="19">
@@ -1098,7 +1098,7 @@
         </is>
       </c>
       <c r="J19" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="20">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="J20" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="21">
@@ -1166,7 +1166,7 @@
         </is>
       </c>
       <c r="J21" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="22">
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="J22" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="23">
@@ -1234,7 +1234,7 @@
         </is>
       </c>
       <c r="J23" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="24">
@@ -1268,7 +1268,7 @@
         </is>
       </c>
       <c r="J24" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="25">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="J25" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="26">
@@ -1336,7 +1336,7 @@
         </is>
       </c>
       <c r="J26" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="27">
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="J27" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="28">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="J28" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="29">
@@ -1438,7 +1438,7 @@
         </is>
       </c>
       <c r="J29" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="30">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="J30" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="31">
@@ -1506,7 +1506,7 @@
         </is>
       </c>
       <c r="J31" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="32">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c r="J32" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="33">
@@ -1574,7 +1574,7 @@
         </is>
       </c>
       <c r="J33" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="34">
@@ -1608,7 +1608,7 @@
         </is>
       </c>
       <c r="J34" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="35">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="J35" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="36">
@@ -1676,7 +1676,7 @@
         </is>
       </c>
       <c r="J36" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="37">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="J37" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="38">
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="J38" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         </is>
       </c>
       <c r="J39" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="40">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="J40" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="41">
@@ -1846,7 +1846,7 @@
         </is>
       </c>
       <c r="J41" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="42">
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="J42" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="43">
@@ -1914,7 +1914,7 @@
         </is>
       </c>
       <c r="J43" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="44">
@@ -1948,7 +1948,7 @@
         </is>
       </c>
       <c r="J44" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="45">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="J45" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="46">
@@ -2016,7 +2016,7 @@
         </is>
       </c>
       <c r="J46" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="47">
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="J47" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="48">
@@ -2084,7 +2084,7 @@
         </is>
       </c>
       <c r="J48" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="49">
@@ -2118,7 +2118,7 @@
         </is>
       </c>
       <c r="J49" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="50">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="J50" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="51">
@@ -2186,7 +2186,7 @@
         </is>
       </c>
       <c r="J51" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="52">
@@ -2220,7 +2220,7 @@
         </is>
       </c>
       <c r="J52" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="53">
@@ -2254,7 +2254,7 @@
         </is>
       </c>
       <c r="J53" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="54">
@@ -2288,7 +2288,7 @@
         </is>
       </c>
       <c r="J54" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="55">
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="J55" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="56">
@@ -2356,7 +2356,7 @@
         </is>
       </c>
       <c r="J56" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="57">
@@ -2390,7 +2390,7 @@
         </is>
       </c>
       <c r="J57" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="58">
@@ -2424,7 +2424,7 @@
         </is>
       </c>
       <c r="J58" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="59">
@@ -2458,7 +2458,7 @@
         </is>
       </c>
       <c r="J59" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="60">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="J60" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="61">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="J61" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="62">
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="J62" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="63">
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="J63" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="64">
@@ -2628,7 +2628,7 @@
         </is>
       </c>
       <c r="J64" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="65">
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="J65" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="66">
@@ -2696,7 +2696,7 @@
         </is>
       </c>
       <c r="J66" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="67">
@@ -2730,7 +2730,7 @@
         </is>
       </c>
       <c r="J67" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="68">
@@ -2764,7 +2764,7 @@
         </is>
       </c>
       <c r="J68" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="69">
@@ -2798,7 +2798,7 @@
         </is>
       </c>
       <c r="J69" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="70">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="J70" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="71">
@@ -2866,7 +2866,7 @@
         </is>
       </c>
       <c r="J71" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="72">
@@ -2900,7 +2900,7 @@
         </is>
       </c>
       <c r="J72" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="73">
@@ -2934,7 +2934,7 @@
         </is>
       </c>
       <c r="J73" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="74">
@@ -2968,7 +2968,7 @@
         </is>
       </c>
       <c r="J74" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="75">
@@ -3002,7 +3002,7 @@
         </is>
       </c>
       <c r="J75" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="76">
@@ -3036,7 +3036,7 @@
         </is>
       </c>
       <c r="J76" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="77">
@@ -3070,7 +3070,7 @@
         </is>
       </c>
       <c r="J77" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="78">
@@ -3104,7 +3104,7 @@
         </is>
       </c>
       <c r="J78" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="79">
@@ -3138,7 +3138,7 @@
         </is>
       </c>
       <c r="J79" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="80">
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="J80" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="81">
@@ -3206,7 +3206,7 @@
         </is>
       </c>
       <c r="J81" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="82">
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="J82" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="83">
@@ -3274,7 +3274,7 @@
         </is>
       </c>
       <c r="J83" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="84">
@@ -3308,7 +3308,7 @@
         </is>
       </c>
       <c r="J84" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="85">
@@ -3342,7 +3342,7 @@
         </is>
       </c>
       <c r="J85" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="86">
@@ -3376,7 +3376,7 @@
         </is>
       </c>
       <c r="J86" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="87">
@@ -3410,7 +3410,7 @@
         </is>
       </c>
       <c r="J87" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="88">
@@ -3444,7 +3444,7 @@
         </is>
       </c>
       <c r="J88" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="89">
@@ -3478,7 +3478,7 @@
         </is>
       </c>
       <c r="J89" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="90">
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="J90" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="91">
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="J91" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="92">
@@ -3580,7 +3580,7 @@
         </is>
       </c>
       <c r="J92" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="93">
@@ -3614,7 +3614,7 @@
         </is>
       </c>
       <c r="J93" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="94">
@@ -3648,7 +3648,7 @@
         </is>
       </c>
       <c r="J94" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="95">
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="J95" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="96">
@@ -3716,7 +3716,7 @@
         </is>
       </c>
       <c r="J96" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="97">
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="J97" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="98">
@@ -3784,7 +3784,7 @@
         </is>
       </c>
       <c r="J98" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="99">
@@ -3818,7 +3818,7 @@
         </is>
       </c>
       <c r="J99" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="100">
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="J100" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="101">
@@ -3886,7 +3886,7 @@
         </is>
       </c>
       <c r="J101" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="102">
@@ -3920,7 +3920,7 @@
         </is>
       </c>
       <c r="J102" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="103">
@@ -3954,7 +3954,7 @@
         </is>
       </c>
       <c r="J103" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="104">
@@ -3988,7 +3988,7 @@
         </is>
       </c>
       <c r="J104" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="105">
@@ -4022,7 +4022,7 @@
         </is>
       </c>
       <c r="J105" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="106">
@@ -4056,7 +4056,7 @@
         </is>
       </c>
       <c r="J106" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="107">
@@ -4090,7 +4090,7 @@
         </is>
       </c>
       <c r="J107" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="108">
@@ -4124,7 +4124,7 @@
         </is>
       </c>
       <c r="J108" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="109">
@@ -4158,7 +4158,7 @@
         </is>
       </c>
       <c r="J109" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="110">
@@ -4192,7 +4192,7 @@
         </is>
       </c>
       <c r="J110" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="111">
@@ -4226,7 +4226,7 @@
         </is>
       </c>
       <c r="J111" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="112">
@@ -4260,7 +4260,7 @@
         </is>
       </c>
       <c r="J112" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="113">
@@ -4294,7 +4294,7 @@
         </is>
       </c>
       <c r="J113" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="114">
@@ -4328,7 +4328,7 @@
         </is>
       </c>
       <c r="J114" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="115">
@@ -4362,7 +4362,7 @@
         </is>
       </c>
       <c r="J115" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="116">
@@ -4396,7 +4396,7 @@
         </is>
       </c>
       <c r="J116" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="117">
@@ -4430,7 +4430,7 @@
         </is>
       </c>
       <c r="J117" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="118">
@@ -4464,7 +4464,7 @@
         </is>
       </c>
       <c r="J118" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="119">
@@ -4498,7 +4498,7 @@
         </is>
       </c>
       <c r="J119" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="120">
@@ -4532,7 +4532,7 @@
         </is>
       </c>
       <c r="J120" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="121">
@@ -4566,7 +4566,7 @@
         </is>
       </c>
       <c r="J121" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="122">
@@ -4600,7 +4600,7 @@
         </is>
       </c>
       <c r="J122" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="123">
@@ -4634,7 +4634,7 @@
         </is>
       </c>
       <c r="J123" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="124">
@@ -4668,7 +4668,7 @@
         </is>
       </c>
       <c r="J124" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="125">
@@ -4702,7 +4702,7 @@
         </is>
       </c>
       <c r="J125" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="126">
@@ -4736,7 +4736,7 @@
         </is>
       </c>
       <c r="J126" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="127">
@@ -4770,7 +4770,7 @@
         </is>
       </c>
       <c r="J127" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="128">
@@ -4804,7 +4804,7 @@
         </is>
       </c>
       <c r="J128" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="129">
@@ -4838,7 +4838,7 @@
         </is>
       </c>
       <c r="J129" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="130">
@@ -4872,7 +4872,7 @@
         </is>
       </c>
       <c r="J130" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="131">
@@ -4906,7 +4906,7 @@
         </is>
       </c>
       <c r="J131" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="132">
@@ -4940,7 +4940,7 @@
         </is>
       </c>
       <c r="J132" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="133">
@@ -4974,7 +4974,7 @@
         </is>
       </c>
       <c r="J133" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="134">
@@ -5008,7 +5008,7 @@
         </is>
       </c>
       <c r="J134" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="135">
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="J135" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="136">
@@ -5076,7 +5076,7 @@
         </is>
       </c>
       <c r="J136" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
     <row r="137">
@@ -5110,7 +5110,7 @@
         </is>
       </c>
       <c r="J137" s="2" t="n">
-        <v>45613.97915358546</v>
+        <v>45614.07711367523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>